<commit_message>
Explicación Tabla de Requerimientos
</commit_message>
<xml_diff>
--- a/Tabla de Requerimientos.xlsx
+++ b/Tabla de Requerimientos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes-my.sharepoint.com/personal/na_angarita1490_uniandes_edu_co/Documents/GerenciaProyectos/Proyecto aplicado en analítica de datos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes-my.sharepoint.com/personal/na_angarita1490_uniandes_edu_co/Documents/GerenciaProyectos/Proyecto aplicado en analítica de datos/Repositorio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="208" documentId="8_{61883769-B994-4E47-B77F-14B90D4D8453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1949D2D8-8439-41A4-8727-095F51D9DB7C}"/>
+  <xr:revisionPtr revIDLastSave="215" documentId="8_{61883769-B994-4E47-B77F-14B90D4D8453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE704328-E113-4A7A-B15D-B36AF5F5B296}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{743D91F9-000F-4CA3-AD1B-C8EE4CDF320F}"/>
+    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{743D91F9-000F-4CA3-AD1B-C8EE4CDF320F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -86,9 +86,6 @@
     <t>R4</t>
   </si>
   <si>
-    <t>Cumple</t>
-  </si>
-  <si>
     <t>R6</t>
   </si>
   <si>
@@ -140,16 +137,10 @@
     <t>Seleccionar mejor algoritmo que permita identificar anomalías.</t>
   </si>
   <si>
-    <t>Revisión</t>
-  </si>
-  <si>
     <t>Métricas de desempeño.</t>
   </si>
   <si>
     <t>Coeficiente de Silhouette más cercano a 1 para algoritmos como PCA, LOF y DBSCAN.</t>
-  </si>
-  <si>
-    <t>Requiere licencia de Power BI</t>
   </si>
   <si>
     <t>Aplicar filtros de fecha, hora, cliente y sector económico para visualizar subgrupos específicos.</t>
@@ -198,10 +189,19 @@
     <t>Dashboard amigable y presentación en demo para los usuarios.</t>
   </si>
   <si>
-    <t>Licencia Power BI.</t>
-  </si>
-  <si>
-    <t>Filtros disponibles para segmentar por clientes y sectores principalmente.</t>
+    <t>Requiere licencia de Power BI.</t>
+  </si>
+  <si>
+    <t>Cumple.</t>
+  </si>
+  <si>
+    <t>Licencia Power BI, cumple.</t>
+  </si>
+  <si>
+    <t>Revisión.</t>
+  </si>
+  <si>
+    <t>Filtros disponibles para segmentar por clientes y sectores principalmente, cumple.</t>
   </si>
 </sst>
 </file>
@@ -633,8 +633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36D44C4E-9805-4040-BB17-C7A7CE9F001B}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A9" zoomScale="90" zoomScaleNormal="70" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="E14" sqref="E13:E14"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="C9" zoomScale="80" zoomScaleNormal="70" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="13"/>
@@ -662,7 +662,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -688,7 +688,7 @@
         <v>8</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="59.25" customHeight="1">
@@ -699,13 +699,13 @@
         <v>10</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="59.25" customHeight="1">
@@ -713,16 +713,16 @@
         <v>12</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="D5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>31</v>
-      </c>
       <c r="E5" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -742,53 +742,53 @@
         <v>13</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="52">
       <c r="A8" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="D8" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F8" s="6"/>
     </row>
     <row r="9" spans="1:6" ht="39">
       <c r="A9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="C9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="D9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>19</v>
-      </c>
       <c r="E9" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -797,67 +797,67 @@
     </row>
     <row r="11" spans="1:6" ht="26">
       <c r="A11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="C11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="D11" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>24</v>
-      </c>
       <c r="E11" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="26">
       <c r="A13" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="D13" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>28</v>
-      </c>
       <c r="E13" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="26">
       <c r="A14" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>53</v>

</xml_diff>